<commit_message>
MZ update cleanData with standardise texts
</commit_message>
<xml_diff>
--- a/examples/rawData/nhanes_dict_2-1.xlsx
+++ b/examples/rawData/nhanes_dict_2-1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/tests/clean/rawData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/examples/rawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="305" documentId="8_{2A74506E-5B93-4425-9454-2A08CB8A3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC67F104-DFD6-492A-9EF6-9D7D93EF3E47}"/>
+  <xr:revisionPtr revIDLastSave="307" documentId="8_{2A74506E-5B93-4425-9454-2A08CB8A3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CD9717-5755-4EBD-955E-EE132ED2D453}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1211,7 +1211,7 @@
   <dimension ref="A1:H78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
MZ 20240403 update bug fixes
</commit_message>
<xml_diff>
--- a/examples/rawData/nhanes_dict_2-1.xlsx
+++ b/examples/rawData/nhanes_dict_2-1.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://itssastar-my.sharepoint.com/personal/tanmz-bii_bii_a-star_edu_sg/Documents/DAR/synData/copula-tabular/examples/rawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="307" documentId="8_{2A74506E-5B93-4425-9454-2A08CB8A3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7CD9717-5755-4EBD-955E-EE132ED2D453}"/>
+  <xr:revisionPtr revIDLastSave="320" documentId="8_{2A74506E-5B93-4425-9454-2A08CB8A3A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59C12F2C-8908-489A-A840-B9F25EFC79B2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$78</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
@@ -295,9 +298,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>0-9; 10-19; 20-29; 30-39; 40-49; 50-59; 60-69; 70+</t>
-  </si>
-  <si>
     <t>Age in months at screening of study participant. Reported for participants aged 0 to 79 years for 2009 to 2010 data. Reported for participants aged 0 to 2 years for 2011 to 2012 data.</t>
   </si>
   <si>
@@ -337,18 +337,9 @@
     <t>A ratio of family income to poverty guidelines. Smaller numbers indicate more poverty.</t>
   </si>
   <si>
-    <t>0-5</t>
-  </si>
-  <si>
     <t>How many rooms are in home of study participant (counting kitchen but not bathroom). 13 rooms = 13 or more rooms.</t>
   </si>
   <si>
-    <t>0-80</t>
-  </si>
-  <si>
-    <t>1-13</t>
-  </si>
-  <si>
     <t>2500, 7500, 12500, 17500, 22500, 30000, 40000, 50000, 60000, 70000, 87500, 100000</t>
   </si>
   <si>
@@ -457,9 +448,6 @@
     <t>Self-reported number of days participant’s mental health was not good out of the past 30 days. Reported for participants aged 12 years or older</t>
   </si>
   <si>
-    <t>0-30</t>
-  </si>
-  <si>
     <t>None; Several; Most; AlmostAll</t>
   </si>
   <si>
@@ -478,27 +466,18 @@
     <t>Age of participant at time of first live birth. 14 years or under = 14, 45 years or older = 45. Reported for female participants aged 20 years or older.</t>
   </si>
   <si>
-    <t>14-45</t>
-  </si>
-  <si>
     <t>Self-reported number of hours study participant usually gets at night on weekdays or workdays. Reported for participants aged 16 years and older.</t>
   </si>
   <si>
     <t>Participant has told a doctor or other health professional that they had trouble sleeping. Reported for participants aged 16 years and older. Coded as Yes or No.</t>
   </si>
   <si>
-    <t>0-12</t>
-  </si>
-  <si>
     <t>Participant does moderate or vigorous-intensity sports, fitness or recreational activities (Yes or No). Reported for participants 12 years or older.</t>
   </si>
   <si>
     <t>Number of days in a typical week that participant does moderate or vigorous-intensity activity. Reported for participants 12 years or older.</t>
   </si>
   <si>
-    <t>1-7</t>
-  </si>
-  <si>
     <t>Number of hours per day on average participant watched TV over the past 30 days. Reported for participants 2 years or older. One of 0_to_1hr, 1_hr, 2_hr, 3_hr, 4_hr, More_4_hr. Not available 2009-2010.</t>
   </si>
   <si>
@@ -506,9 +485,6 @@
   </si>
   <si>
     <t>0_hrs; 0_to_1_hr; 1_hr; 2_hr; 3_hr; 4_hr; More_4_hr</t>
-  </si>
-  <si>
-    <t>0-6</t>
   </si>
   <si>
     <t>Participant has consumed at least 12 drinks of any type of alcoholic beverage in any one year. Reported for participants 18 years or older as Yes or No.</t>
@@ -779,6 +755,33 @@
   </si>
   <si>
     <t>TESTID</t>
+  </si>
+  <si>
+    <t>[0,80]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-9; 10-19; 20-29; 30-39; 40-49; 50-59; 60-69; 70+</t>
+  </si>
+  <si>
+    <t>[0,5]</t>
+  </si>
+  <si>
+    <t>[1,13]</t>
+  </si>
+  <si>
+    <t>[0,30]</t>
+  </si>
+  <si>
+    <t>[14,45]</t>
+  </si>
+  <si>
+    <t>[0,12]</t>
+  </si>
+  <si>
+    <t>[1,7]</t>
+  </si>
+  <si>
+    <t>[0,6]</t>
   </si>
 </sst>
 </file>
@@ -888,9 +891,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -928,9 +931,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -963,26 +966,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1015,26 +1001,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1208,10 +1177,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1250,7 +1220,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1261,7 +1231,7 @@
         <v>81</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1269,19 +1239,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1301,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1315,13 +1285,13 @@
         <v>86</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F5" s="2">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1335,16 +1305,16 @@
         <v>81</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>107</v>
+        <v>227</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F6" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1355,10 +1325,10 @@
         <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>91</v>
+        <v>228</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -1367,142 +1337,142 @@
         <v>90</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F8" s="2">
         <v>5</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F9" s="2">
         <v>6</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F10" s="2">
         <v>7</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F11" s="2">
         <v>8</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>100</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F12" s="2">
         <v>9</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F13" s="2">
         <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1510,16 +1480,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F14" s="2">
         <v>11</v>
@@ -1528,7 +1498,7 @@
         <v>90</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1536,22 +1506,22 @@
         <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>229</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F15" s="2">
         <v>12</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1559,45 +1529,45 @@
         <v>18</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="F16" s="2">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F17" s="2">
         <v>14</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -1605,16 +1575,16 @@
         <v>82</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F18" s="2">
         <v>15</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1622,13 +1592,13 @@
         <v>21</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F19" s="2">
         <v>16</v>
@@ -1639,19 +1609,19 @@
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F20" s="2">
         <v>17</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1659,19 +1629,19 @@
         <v>23</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F21" s="2">
         <v>18</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1679,19 +1649,19 @@
         <v>24</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F22" s="2">
         <v>19</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1699,13 +1669,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F23" s="2">
         <v>20</v>
@@ -1714,24 +1684,24 @@
         <v>90</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F24" s="2">
         <v>21</v>
@@ -1740,24 +1710,24 @@
         <v>90</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F25" s="2">
         <v>22</v>
@@ -1766,7 +1736,7 @@
         <v>90</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1774,13 +1744,13 @@
         <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F26" s="2">
         <v>23</v>
@@ -1791,13 +1761,13 @@
         <v>29</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F27" s="2">
         <v>24</v>
@@ -1808,13 +1778,13 @@
         <v>30</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F28" s="2">
         <v>25</v>
@@ -1825,13 +1795,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F29" s="2">
         <v>26</v>
@@ -1842,13 +1812,13 @@
         <v>32</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F30" s="2">
         <v>27</v>
@@ -1859,13 +1829,13 @@
         <v>33</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F31" s="2">
         <v>28</v>
@@ -1876,13 +1846,13 @@
         <v>34</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F32" s="2">
         <v>29</v>
@@ -1893,13 +1863,13 @@
         <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F33" s="2">
         <v>30</v>
@@ -1910,13 +1880,13 @@
         <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F34" s="2">
         <v>31</v>
@@ -1927,19 +1897,19 @@
         <v>37</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F35" s="2">
         <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1947,19 +1917,19 @@
         <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F36" s="2">
         <v>33</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1967,19 +1937,19 @@
         <v>39</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F37" s="2">
         <v>34</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1987,19 +1957,19 @@
         <v>40</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F38" s="2">
         <v>35</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2007,19 +1977,19 @@
         <v>41</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F39" s="2">
         <v>36</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2027,19 +1997,19 @@
         <v>42</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F40" s="2">
         <v>37</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2047,42 +2017,42 @@
         <v>43</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F41" s="2">
         <v>38</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F42" s="2">
         <v>39</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2090,42 +2060,42 @@
         <v>45</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F43" s="2">
         <v>40</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F44" s="2">
         <v>41</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2133,22 +2103,22 @@
         <v>47</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F45" s="2">
         <v>42</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2156,68 +2126,68 @@
         <v>48</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>145</v>
+        <v>231</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F46" s="2">
         <v>43</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F47" s="2">
         <v>44</v>
       </c>
       <c r="H47" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F48" s="2">
         <v>45</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2225,19 +2195,19 @@
         <v>51</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F49" s="2">
         <v>46</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2245,19 +2215,19 @@
         <v>52</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F50" s="2">
         <v>47</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="72" x14ac:dyDescent="0.3">
@@ -2265,22 +2235,22 @@
         <v>53</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>152</v>
+        <v>232</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F51" s="2">
         <v>48</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2288,68 +2258,68 @@
         <v>54</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F52" s="2">
         <v>49</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F53" s="2">
         <v>50</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F54" s="2">
         <v>51</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2357,68 +2327,68 @@
         <v>57</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>158</v>
+        <v>234</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F55" s="2">
         <v>52</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F56" s="2">
         <v>53</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F57" s="2">
         <v>54</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2426,22 +2396,22 @@
         <v>60</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>162</v>
+        <v>235</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F58" s="2">
         <v>55</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2449,45 +2419,45 @@
         <v>61</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>81</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>162</v>
+        <v>235</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F59" s="2">
         <v>56</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F60" s="2">
         <v>57</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2495,19 +2465,19 @@
         <v>63</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F61" s="2">
         <v>58</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2515,68 +2485,68 @@
         <v>64</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F62" s="2">
         <v>59</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F63" s="2">
         <v>60</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F64" s="2">
         <v>61</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>67</v>
       </c>
@@ -2584,10 +2554,10 @@
         <v>82</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F65" s="2">
         <v>62</v>
@@ -2596,7 +2566,7 @@
         <v>90</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2604,42 +2574,42 @@
         <v>68</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F66" s="2">
         <v>63</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F67" s="2">
         <v>64</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2647,42 +2617,42 @@
         <v>70</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F68" s="2">
         <v>65</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>71</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F69" s="2">
         <v>66</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2690,65 +2660,65 @@
         <v>72</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F70" s="2">
         <v>67</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F71" s="2">
         <v>68</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F72" s="2">
         <v>69</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
@@ -2756,19 +2726,19 @@
         <v>75</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F73" s="2">
         <v>70</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2776,19 +2746,19 @@
         <v>76</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F74" s="2">
         <v>71</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -2796,91 +2766,98 @@
         <v>77</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>81</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F75" s="2">
         <v>72</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F76" s="2">
         <v>73</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="F77" s="2">
         <v>74</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="42.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>80</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="F78" s="2">
         <v>75</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H78" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="numeric"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>